<commit_message>
Acrescentando atributos para classe tecido
Atributos necessários para que consiga fazer a conexão com outro API
</commit_message>
<xml_diff>
--- a/src/main/resources/planilhanova.xlsx
+++ b/src/main/resources/planilhanova.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\novo-teste-excel\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\importacao-dados-planilha-excel\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058E0945-5DDC-46A1-A1F6-96D4FB734F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C87110-0596-40CD-9BC8-8FA51D8595C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,27 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>NP</t>
+    <t>Universal</t>
   </si>
   <si>
-    <t>Universal</t>
+    <t>AS</t>
   </si>
   <si>
     <t>1009</t>
   </si>
   <si>
-    <t>Unicolor</t>
-  </si>
-  <si>
-    <t>5414</t>
-  </si>
-  <si>
-    <t>Agil</t>
-  </si>
-  <si>
-    <t>AS</t>
+    <t>np</t>
   </si>
 </sst>
 </file>
@@ -364,61 +355,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>189598</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>59.3</v>
-      </c>
       <c r="E1">
+        <v>59</v>
+      </c>
+      <c r="F1">
         <v>2</v>
       </c>
-      <c r="F1">
-        <v>781298</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1">
+        <v>781228</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>65</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>798532</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deletando arquivos e configurando atributos
Deletando as planilhas que foram utilizadas para testes e já não tem mais utilidades. Configuração dos formatos dos atributos e a utilização deles na classe de importação.
</commit_message>
<xml_diff>
--- a/src/main/resources/planilhanova.xlsx
+++ b/src/main/resources/planilhanova.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\importacao-dados-planilha-excel\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C87110-0596-40CD-9BC8-8FA51D8595C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D1E0D4-728E-4059-B8FB-DD2E936CE886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5910" yWindow="285" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Universal</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>np</t>
+  </si>
+  <si>
+    <t>02/03/2024</t>
   </si>
 </sst>
 </file>
@@ -72,9 +75,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,15 +359,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>189598</v>
       </c>
@@ -380,12 +387,24 @@
         <v>59</v>
       </c>
       <c r="F1">
+        <v>1.65</v>
+      </c>
+      <c r="G1">
         <v>2</v>
       </c>
-      <c r="G1">
+      <c r="H1">
+        <v>9.56</v>
+      </c>
+      <c r="I1">
+        <v>1526</v>
+      </c>
+      <c r="J1">
         <v>781228</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>